<commit_message>
Add default esqlabs data importer Value
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/NewProject/ProjectConfiguration.xlsx
+++ b/inst/extdata/examples/NewProject/ProjectConfiguration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\NewProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBF1067-13CD-4C88-B89C-43796F809540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24A8370-5932-4580-A7C6-A341BEB5087B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7575" yWindow="2475" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Property</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Models</t>
+  </si>
+  <si>
+    <t>esqlabs_dataImporter_configuration.xml</t>
   </si>
 </sst>
 </file>
@@ -471,7 +474,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,6 +606,9 @@
       <c r="A12" t="s">
         <v>22</v>
       </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
       <c r="C12" t="s">
         <v>27</v>
       </c>
@@ -633,6 +639,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6d50ae52c45ae5cf3a9b42a45f9049e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f65cf74c317ca0ec831fcb171d38ef6f" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -849,12 +861,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -865,6 +871,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7732FB-5A16-4D8D-B2A0-DAE82353628B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CE9E921-488E-4950-83CF-BA07CBEDBDF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -883,15 +898,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7732FB-5A16-4D8D-B2A0-DAE82353628B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B48AA3D9-A829-4D13-95B1-181AC8A856B4}">
   <ds:schemaRefs>

</xml_diff>